<commit_message>
Add function for the app to be able accept .pdf format
</commit_message>
<xml_diff>
--- a/ocr-receipt-test/output.xlsx
+++ b/ocr-receipt-test/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,100 @@
           <t>THE BREAKFAST CLUB</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>258</t>
-        </is>
+      <c r="B2" t="n">
+        <v>258</v>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>13.32</t>
-        </is>
+      <c r="D2" t="n">
+        <v>13.32</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>5000 NORTH ALAMAR AVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>THE BREAKFAST CLUB</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>258</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>13.32</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5000 NORTH ALAMAR AVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Montana Restaurant.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10/07/2020</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>36.98</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>6542 MAGNOLIA LAKE COURT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HARBOR LANE CAFE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11/20/2019</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>31.39</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3941 GREEN OAKS BLVD</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HARBOR LANE CAFE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11/20/2019</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>31.39</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3941 GREEN OAKS BLVD</t>
         </is>
       </c>
     </row>

</xml_diff>